<commit_message>
Se modifico el inventario del lab03
</commit_message>
<xml_diff>
--- a/lab03/Libro1.xlsx
+++ b/lab03/Libro1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reposInventario2025\lab03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recuperado\reposInventario2025\lab03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E2C61B-B2E5-46F9-B159-5D8C979CF92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3852AF-F094-4BED-A99F-94ED6BC3738F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4770" yWindow="2445" windowWidth="21600" windowHeight="11295" xr2:uid="{2CBF6FFA-8719-440B-9FC5-C5276456B4AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2CBF6FFA-8719-440B-9FC5-C5276456B4AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
     <t>l003</t>
   </si>
   <si>
-    <t>PC DELL ALL IN ONE CORE I9</t>
+    <t>PC DELL ALL IN ONE CORE I9 mem 32gb</t>
   </si>
 </sst>
 </file>
@@ -437,12 +437,12 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="340" zoomScaleNormal="340" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>